<commit_message>
Updating JSON files of run 10
</commit_message>
<xml_diff>
--- a/scripts/sari/new_data.xlsx
+++ b/scripts/sari/new_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
+    <workbookView xWindow="520" yWindow="20" windowWidth="28720" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="new_data.tsv.txt" sheetId="1" r:id="rId1"/>
@@ -803,10 +803,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -958,7 +959,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1198,11 +1199,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1318,6 +1427,30 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1466,11 +1599,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102928472"/>
-        <c:axId val="2102931896"/>
+        <c:axId val="2088124792"/>
+        <c:axId val="2088128088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102928472"/>
+        <c:axId val="2088124792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,12 +1638,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102931896"/>
+        <c:crossAx val="2088128088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102931896"/>
+        <c:axId val="2088128088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,7 +1688,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2102928472"/>
+        <c:crossAx val="2088124792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1791,11 +1924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103006840"/>
-        <c:axId val="2103010040"/>
+        <c:axId val="2087749976"/>
+        <c:axId val="2087753272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103006840"/>
+        <c:axId val="2087749976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,12 +1963,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103010040"/>
+        <c:crossAx val="2087753272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103010040"/>
+        <c:axId val="2087753272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +2013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103006840"/>
+        <c:crossAx val="2087749976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2108,11 +2241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103051912"/>
-        <c:axId val="2103055128"/>
+        <c:axId val="2087794584"/>
+        <c:axId val="2087797896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103051912"/>
+        <c:axId val="2087794584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,12 +2280,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103055128"/>
+        <c:crossAx val="2087797896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103055128"/>
+        <c:axId val="2087797896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,7 +2330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103051912"/>
+        <c:crossAx val="2087794584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2427,11 +2560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103098856"/>
-        <c:axId val="2103102056"/>
+        <c:axId val="2087840392"/>
+        <c:axId val="2087843688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103098856"/>
+        <c:axId val="2087840392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,12 +2599,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103102056"/>
+        <c:crossAx val="2087843688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103102056"/>
+        <c:axId val="2087843688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2516,7 +2649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103098856"/>
+        <c:crossAx val="2087840392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3047,11 +3180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FC97"/>
+  <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC64" sqref="AC64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3072,7 +3205,7 @@
     <col min="20" max="21" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3155,7 +3288,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:159" s="5" customFormat="1">
+    <row r="2" spans="1:28" s="5" customFormat="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3200,7 +3333,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:159" s="5" customFormat="1">
+    <row r="3" spans="1:28" s="5" customFormat="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3245,7 +3378,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:159" s="5" customFormat="1">
+    <row r="4" spans="1:28" s="5" customFormat="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3290,7 +3423,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:159" s="5" customFormat="1">
+    <row r="5" spans="1:28" s="5" customFormat="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3335,7 +3468,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:159" s="5" customFormat="1">
+    <row r="6" spans="1:28" s="5" customFormat="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3380,7 +3513,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:159" s="5" customFormat="1">
+    <row r="7" spans="1:28" s="5" customFormat="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3425,7 +3558,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:159" s="5" customFormat="1">
+    <row r="8" spans="1:28" s="5" customFormat="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3470,7 +3603,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:159" s="5" customFormat="1">
+    <row r="9" spans="1:28" s="5" customFormat="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3515,7 +3648,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:159" s="5" customFormat="1">
+    <row r="10" spans="1:28" s="5" customFormat="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3560,7 +3693,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:159" s="5" customFormat="1">
+    <row r="11" spans="1:28" s="5" customFormat="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3617,139 +3750,8 @@
       <c r="Z11"/>
       <c r="AA11"/>
       <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AG11"/>
-      <c r="AH11"/>
-      <c r="AI11"/>
-      <c r="AJ11"/>
-      <c r="AK11"/>
-      <c r="AL11"/>
-      <c r="AM11"/>
-      <c r="AN11"/>
-      <c r="AO11"/>
-      <c r="AP11"/>
-      <c r="AQ11"/>
-      <c r="AR11"/>
-      <c r="AS11"/>
-      <c r="AT11"/>
-      <c r="AU11"/>
-      <c r="AV11"/>
-      <c r="AW11"/>
-      <c r="AX11"/>
-      <c r="AY11"/>
-      <c r="AZ11"/>
-      <c r="BA11"/>
-      <c r="BB11"/>
-      <c r="BC11"/>
-      <c r="BD11"/>
-      <c r="BE11"/>
-      <c r="BF11"/>
-      <c r="BG11"/>
-      <c r="BH11"/>
-      <c r="BI11"/>
-      <c r="BJ11"/>
-      <c r="BK11"/>
-      <c r="BL11"/>
-      <c r="BM11"/>
-      <c r="BN11"/>
-      <c r="BO11"/>
-      <c r="BP11"/>
-      <c r="BQ11"/>
-      <c r="BR11"/>
-      <c r="BS11"/>
-      <c r="BT11"/>
-      <c r="BU11"/>
-      <c r="BV11"/>
-      <c r="BW11"/>
-      <c r="BX11"/>
-      <c r="BY11"/>
-      <c r="BZ11"/>
-      <c r="CA11"/>
-      <c r="CB11"/>
-      <c r="CC11"/>
-      <c r="CD11"/>
-      <c r="CE11"/>
-      <c r="CF11"/>
-      <c r="CG11"/>
-      <c r="CH11"/>
-      <c r="CI11"/>
-      <c r="CJ11"/>
-      <c r="CK11"/>
-      <c r="CL11"/>
-      <c r="CM11"/>
-      <c r="CN11"/>
-      <c r="CO11"/>
-      <c r="CP11"/>
-      <c r="CQ11"/>
-      <c r="CR11"/>
-      <c r="CS11"/>
-      <c r="CT11"/>
-      <c r="CU11"/>
-      <c r="CV11"/>
-      <c r="CW11"/>
-      <c r="CX11"/>
-      <c r="CY11"/>
-      <c r="CZ11"/>
-      <c r="DA11"/>
-      <c r="DB11"/>
-      <c r="DC11"/>
-      <c r="DD11"/>
-      <c r="DE11"/>
-      <c r="DF11"/>
-      <c r="DG11"/>
-      <c r="DH11"/>
-      <c r="DI11"/>
-      <c r="DJ11"/>
-      <c r="DK11"/>
-      <c r="DL11"/>
-      <c r="DM11"/>
-      <c r="DN11"/>
-      <c r="DO11"/>
-      <c r="DP11"/>
-      <c r="DQ11"/>
-      <c r="DR11"/>
-      <c r="DS11"/>
-      <c r="DT11"/>
-      <c r="DU11"/>
-      <c r="DV11"/>
-      <c r="DW11"/>
-      <c r="DX11"/>
-      <c r="DY11"/>
-      <c r="DZ11"/>
-      <c r="EA11"/>
-      <c r="EB11"/>
-      <c r="EC11"/>
-      <c r="ED11"/>
-      <c r="EE11"/>
-      <c r="EF11"/>
-      <c r="EG11"/>
-      <c r="EH11"/>
-      <c r="EI11"/>
-      <c r="EJ11"/>
-      <c r="EK11"/>
-      <c r="EL11"/>
-      <c r="EM11"/>
-      <c r="EN11"/>
-      <c r="EO11"/>
-      <c r="EP11"/>
-      <c r="EQ11"/>
-      <c r="ER11"/>
-      <c r="ES11"/>
-      <c r="ET11"/>
-      <c r="EU11"/>
-      <c r="EV11"/>
-      <c r="EW11"/>
-      <c r="EX11"/>
-      <c r="EY11"/>
-      <c r="EZ11"/>
-      <c r="FA11"/>
-      <c r="FB11"/>
-      <c r="FC11"/>
-    </row>
-    <row r="12" spans="1:159" s="5" customFormat="1">
+    </row>
+    <row r="12" spans="1:28" s="5" customFormat="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3806,139 +3808,8 @@
       <c r="Z12"/>
       <c r="AA12"/>
       <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-      <c r="AH12"/>
-      <c r="AI12"/>
-      <c r="AJ12"/>
-      <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
-      <c r="AN12"/>
-      <c r="AO12"/>
-      <c r="AP12"/>
-      <c r="AQ12"/>
-      <c r="AR12"/>
-      <c r="AS12"/>
-      <c r="AT12"/>
-      <c r="AU12"/>
-      <c r="AV12"/>
-      <c r="AW12"/>
-      <c r="AX12"/>
-      <c r="AY12"/>
-      <c r="AZ12"/>
-      <c r="BA12"/>
-      <c r="BB12"/>
-      <c r="BC12"/>
-      <c r="BD12"/>
-      <c r="BE12"/>
-      <c r="BF12"/>
-      <c r="BG12"/>
-      <c r="BH12"/>
-      <c r="BI12"/>
-      <c r="BJ12"/>
-      <c r="BK12"/>
-      <c r="BL12"/>
-      <c r="BM12"/>
-      <c r="BN12"/>
-      <c r="BO12"/>
-      <c r="BP12"/>
-      <c r="BQ12"/>
-      <c r="BR12"/>
-      <c r="BS12"/>
-      <c r="BT12"/>
-      <c r="BU12"/>
-      <c r="BV12"/>
-      <c r="BW12"/>
-      <c r="BX12"/>
-      <c r="BY12"/>
-      <c r="BZ12"/>
-      <c r="CA12"/>
-      <c r="CB12"/>
-      <c r="CC12"/>
-      <c r="CD12"/>
-      <c r="CE12"/>
-      <c r="CF12"/>
-      <c r="CG12"/>
-      <c r="CH12"/>
-      <c r="CI12"/>
-      <c r="CJ12"/>
-      <c r="CK12"/>
-      <c r="CL12"/>
-      <c r="CM12"/>
-      <c r="CN12"/>
-      <c r="CO12"/>
-      <c r="CP12"/>
-      <c r="CQ12"/>
-      <c r="CR12"/>
-      <c r="CS12"/>
-      <c r="CT12"/>
-      <c r="CU12"/>
-      <c r="CV12"/>
-      <c r="CW12"/>
-      <c r="CX12"/>
-      <c r="CY12"/>
-      <c r="CZ12"/>
-      <c r="DA12"/>
-      <c r="DB12"/>
-      <c r="DC12"/>
-      <c r="DD12"/>
-      <c r="DE12"/>
-      <c r="DF12"/>
-      <c r="DG12"/>
-      <c r="DH12"/>
-      <c r="DI12"/>
-      <c r="DJ12"/>
-      <c r="DK12"/>
-      <c r="DL12"/>
-      <c r="DM12"/>
-      <c r="DN12"/>
-      <c r="DO12"/>
-      <c r="DP12"/>
-      <c r="DQ12"/>
-      <c r="DR12"/>
-      <c r="DS12"/>
-      <c r="DT12"/>
-      <c r="DU12"/>
-      <c r="DV12"/>
-      <c r="DW12"/>
-      <c r="DX12"/>
-      <c r="DY12"/>
-      <c r="DZ12"/>
-      <c r="EA12"/>
-      <c r="EB12"/>
-      <c r="EC12"/>
-      <c r="ED12"/>
-      <c r="EE12"/>
-      <c r="EF12"/>
-      <c r="EG12"/>
-      <c r="EH12"/>
-      <c r="EI12"/>
-      <c r="EJ12"/>
-      <c r="EK12"/>
-      <c r="EL12"/>
-      <c r="EM12"/>
-      <c r="EN12"/>
-      <c r="EO12"/>
-      <c r="EP12"/>
-      <c r="EQ12"/>
-      <c r="ER12"/>
-      <c r="ES12"/>
-      <c r="ET12"/>
-      <c r="EU12"/>
-      <c r="EV12"/>
-      <c r="EW12"/>
-      <c r="EX12"/>
-      <c r="EY12"/>
-      <c r="EZ12"/>
-      <c r="FA12"/>
-      <c r="FB12"/>
-      <c r="FC12"/>
-    </row>
-    <row r="13" spans="1:159" s="5" customFormat="1">
+    </row>
+    <row r="13" spans="1:28" s="5" customFormat="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3995,139 +3866,8 @@
       <c r="Z13"/>
       <c r="AA13"/>
       <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-      <c r="AE13"/>
-      <c r="AF13"/>
-      <c r="AG13"/>
-      <c r="AH13"/>
-      <c r="AI13"/>
-      <c r="AJ13"/>
-      <c r="AK13"/>
-      <c r="AL13"/>
-      <c r="AM13"/>
-      <c r="AN13"/>
-      <c r="AO13"/>
-      <c r="AP13"/>
-      <c r="AQ13"/>
-      <c r="AR13"/>
-      <c r="AS13"/>
-      <c r="AT13"/>
-      <c r="AU13"/>
-      <c r="AV13"/>
-      <c r="AW13"/>
-      <c r="AX13"/>
-      <c r="AY13"/>
-      <c r="AZ13"/>
-      <c r="BA13"/>
-      <c r="BB13"/>
-      <c r="BC13"/>
-      <c r="BD13"/>
-      <c r="BE13"/>
-      <c r="BF13"/>
-      <c r="BG13"/>
-      <c r="BH13"/>
-      <c r="BI13"/>
-      <c r="BJ13"/>
-      <c r="BK13"/>
-      <c r="BL13"/>
-      <c r="BM13"/>
-      <c r="BN13"/>
-      <c r="BO13"/>
-      <c r="BP13"/>
-      <c r="BQ13"/>
-      <c r="BR13"/>
-      <c r="BS13"/>
-      <c r="BT13"/>
-      <c r="BU13"/>
-      <c r="BV13"/>
-      <c r="BW13"/>
-      <c r="BX13"/>
-      <c r="BY13"/>
-      <c r="BZ13"/>
-      <c r="CA13"/>
-      <c r="CB13"/>
-      <c r="CC13"/>
-      <c r="CD13"/>
-      <c r="CE13"/>
-      <c r="CF13"/>
-      <c r="CG13"/>
-      <c r="CH13"/>
-      <c r="CI13"/>
-      <c r="CJ13"/>
-      <c r="CK13"/>
-      <c r="CL13"/>
-      <c r="CM13"/>
-      <c r="CN13"/>
-      <c r="CO13"/>
-      <c r="CP13"/>
-      <c r="CQ13"/>
-      <c r="CR13"/>
-      <c r="CS13"/>
-      <c r="CT13"/>
-      <c r="CU13"/>
-      <c r="CV13"/>
-      <c r="CW13"/>
-      <c r="CX13"/>
-      <c r="CY13"/>
-      <c r="CZ13"/>
-      <c r="DA13"/>
-      <c r="DB13"/>
-      <c r="DC13"/>
-      <c r="DD13"/>
-      <c r="DE13"/>
-      <c r="DF13"/>
-      <c r="DG13"/>
-      <c r="DH13"/>
-      <c r="DI13"/>
-      <c r="DJ13"/>
-      <c r="DK13"/>
-      <c r="DL13"/>
-      <c r="DM13"/>
-      <c r="DN13"/>
-      <c r="DO13"/>
-      <c r="DP13"/>
-      <c r="DQ13"/>
-      <c r="DR13"/>
-      <c r="DS13"/>
-      <c r="DT13"/>
-      <c r="DU13"/>
-      <c r="DV13"/>
-      <c r="DW13"/>
-      <c r="DX13"/>
-      <c r="DY13"/>
-      <c r="DZ13"/>
-      <c r="EA13"/>
-      <c r="EB13"/>
-      <c r="EC13"/>
-      <c r="ED13"/>
-      <c r="EE13"/>
-      <c r="EF13"/>
-      <c r="EG13"/>
-      <c r="EH13"/>
-      <c r="EI13"/>
-      <c r="EJ13"/>
-      <c r="EK13"/>
-      <c r="EL13"/>
-      <c r="EM13"/>
-      <c r="EN13"/>
-      <c r="EO13"/>
-      <c r="EP13"/>
-      <c r="EQ13"/>
-      <c r="ER13"/>
-      <c r="ES13"/>
-      <c r="ET13"/>
-      <c r="EU13"/>
-      <c r="EV13"/>
-      <c r="EW13"/>
-      <c r="EX13"/>
-      <c r="EY13"/>
-      <c r="EZ13"/>
-      <c r="FA13"/>
-      <c r="FB13"/>
-      <c r="FC13"/>
-    </row>
-    <row r="14" spans="1:159" s="5" customFormat="1">
+    </row>
+    <row r="14" spans="1:28" s="5" customFormat="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4184,139 +3924,8 @@
       <c r="Z14"/>
       <c r="AA14"/>
       <c r="AB14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
-      <c r="AE14"/>
-      <c r="AF14"/>
-      <c r="AG14"/>
-      <c r="AH14"/>
-      <c r="AI14"/>
-      <c r="AJ14"/>
-      <c r="AK14"/>
-      <c r="AL14"/>
-      <c r="AM14"/>
-      <c r="AN14"/>
-      <c r="AO14"/>
-      <c r="AP14"/>
-      <c r="AQ14"/>
-      <c r="AR14"/>
-      <c r="AS14"/>
-      <c r="AT14"/>
-      <c r="AU14"/>
-      <c r="AV14"/>
-      <c r="AW14"/>
-      <c r="AX14"/>
-      <c r="AY14"/>
-      <c r="AZ14"/>
-      <c r="BA14"/>
-      <c r="BB14"/>
-      <c r="BC14"/>
-      <c r="BD14"/>
-      <c r="BE14"/>
-      <c r="BF14"/>
-      <c r="BG14"/>
-      <c r="BH14"/>
-      <c r="BI14"/>
-      <c r="BJ14"/>
-      <c r="BK14"/>
-      <c r="BL14"/>
-      <c r="BM14"/>
-      <c r="BN14"/>
-      <c r="BO14"/>
-      <c r="BP14"/>
-      <c r="BQ14"/>
-      <c r="BR14"/>
-      <c r="BS14"/>
-      <c r="BT14"/>
-      <c r="BU14"/>
-      <c r="BV14"/>
-      <c r="BW14"/>
-      <c r="BX14"/>
-      <c r="BY14"/>
-      <c r="BZ14"/>
-      <c r="CA14"/>
-      <c r="CB14"/>
-      <c r="CC14"/>
-      <c r="CD14"/>
-      <c r="CE14"/>
-      <c r="CF14"/>
-      <c r="CG14"/>
-      <c r="CH14"/>
-      <c r="CI14"/>
-      <c r="CJ14"/>
-      <c r="CK14"/>
-      <c r="CL14"/>
-      <c r="CM14"/>
-      <c r="CN14"/>
-      <c r="CO14"/>
-      <c r="CP14"/>
-      <c r="CQ14"/>
-      <c r="CR14"/>
-      <c r="CS14"/>
-      <c r="CT14"/>
-      <c r="CU14"/>
-      <c r="CV14"/>
-      <c r="CW14"/>
-      <c r="CX14"/>
-      <c r="CY14"/>
-      <c r="CZ14"/>
-      <c r="DA14"/>
-      <c r="DB14"/>
-      <c r="DC14"/>
-      <c r="DD14"/>
-      <c r="DE14"/>
-      <c r="DF14"/>
-      <c r="DG14"/>
-      <c r="DH14"/>
-      <c r="DI14"/>
-      <c r="DJ14"/>
-      <c r="DK14"/>
-      <c r="DL14"/>
-      <c r="DM14"/>
-      <c r="DN14"/>
-      <c r="DO14"/>
-      <c r="DP14"/>
-      <c r="DQ14"/>
-      <c r="DR14"/>
-      <c r="DS14"/>
-      <c r="DT14"/>
-      <c r="DU14"/>
-      <c r="DV14"/>
-      <c r="DW14"/>
-      <c r="DX14"/>
-      <c r="DY14"/>
-      <c r="DZ14"/>
-      <c r="EA14"/>
-      <c r="EB14"/>
-      <c r="EC14"/>
-      <c r="ED14"/>
-      <c r="EE14"/>
-      <c r="EF14"/>
-      <c r="EG14"/>
-      <c r="EH14"/>
-      <c r="EI14"/>
-      <c r="EJ14"/>
-      <c r="EK14"/>
-      <c r="EL14"/>
-      <c r="EM14"/>
-      <c r="EN14"/>
-      <c r="EO14"/>
-      <c r="EP14"/>
-      <c r="EQ14"/>
-      <c r="ER14"/>
-      <c r="ES14"/>
-      <c r="ET14"/>
-      <c r="EU14"/>
-      <c r="EV14"/>
-      <c r="EW14"/>
-      <c r="EX14"/>
-      <c r="EY14"/>
-      <c r="EZ14"/>
-      <c r="FA14"/>
-      <c r="FB14"/>
-      <c r="FC14"/>
-    </row>
-    <row r="15" spans="1:159" s="3" customFormat="1">
+    </row>
+    <row r="15" spans="1:28" s="3" customFormat="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -4374,139 +3983,8 @@
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
-      <c r="AC15"/>
-      <c r="AD15"/>
-      <c r="AE15"/>
-      <c r="AF15"/>
-      <c r="AG15"/>
-      <c r="AH15"/>
-      <c r="AI15"/>
-      <c r="AJ15"/>
-      <c r="AK15"/>
-      <c r="AL15"/>
-      <c r="AM15"/>
-      <c r="AN15"/>
-      <c r="AO15"/>
-      <c r="AP15"/>
-      <c r="AQ15"/>
-      <c r="AR15"/>
-      <c r="AS15"/>
-      <c r="AT15"/>
-      <c r="AU15"/>
-      <c r="AV15"/>
-      <c r="AW15"/>
-      <c r="AX15"/>
-      <c r="AY15"/>
-      <c r="AZ15"/>
-      <c r="BA15"/>
-      <c r="BB15"/>
-      <c r="BC15"/>
-      <c r="BD15"/>
-      <c r="BE15"/>
-      <c r="BF15"/>
-      <c r="BG15"/>
-      <c r="BH15"/>
-      <c r="BI15"/>
-      <c r="BJ15"/>
-      <c r="BK15"/>
-      <c r="BL15"/>
-      <c r="BM15"/>
-      <c r="BN15"/>
-      <c r="BO15"/>
-      <c r="BP15"/>
-      <c r="BQ15"/>
-      <c r="BR15"/>
-      <c r="BS15"/>
-      <c r="BT15"/>
-      <c r="BU15"/>
-      <c r="BV15"/>
-      <c r="BW15"/>
-      <c r="BX15"/>
-      <c r="BY15"/>
-      <c r="BZ15"/>
-      <c r="CA15"/>
-      <c r="CB15"/>
-      <c r="CC15"/>
-      <c r="CD15"/>
-      <c r="CE15"/>
-      <c r="CF15"/>
-      <c r="CG15"/>
-      <c r="CH15"/>
-      <c r="CI15"/>
-      <c r="CJ15"/>
-      <c r="CK15"/>
-      <c r="CL15"/>
-      <c r="CM15"/>
-      <c r="CN15"/>
-      <c r="CO15"/>
-      <c r="CP15"/>
-      <c r="CQ15"/>
-      <c r="CR15"/>
-      <c r="CS15"/>
-      <c r="CT15"/>
-      <c r="CU15"/>
-      <c r="CV15"/>
-      <c r="CW15"/>
-      <c r="CX15"/>
-      <c r="CY15"/>
-      <c r="CZ15"/>
-      <c r="DA15"/>
-      <c r="DB15"/>
-      <c r="DC15"/>
-      <c r="DD15"/>
-      <c r="DE15"/>
-      <c r="DF15"/>
-      <c r="DG15"/>
-      <c r="DH15"/>
-      <c r="DI15"/>
-      <c r="DJ15"/>
-      <c r="DK15"/>
-      <c r="DL15"/>
-      <c r="DM15"/>
-      <c r="DN15"/>
-      <c r="DO15"/>
-      <c r="DP15"/>
-      <c r="DQ15"/>
-      <c r="DR15"/>
-      <c r="DS15"/>
-      <c r="DT15"/>
-      <c r="DU15"/>
-      <c r="DV15"/>
-      <c r="DW15"/>
-      <c r="DX15"/>
-      <c r="DY15"/>
-      <c r="DZ15"/>
-      <c r="EA15"/>
-      <c r="EB15"/>
-      <c r="EC15"/>
-      <c r="ED15"/>
-      <c r="EE15"/>
-      <c r="EF15"/>
-      <c r="EG15"/>
-      <c r="EH15"/>
-      <c r="EI15"/>
-      <c r="EJ15"/>
-      <c r="EK15"/>
-      <c r="EL15"/>
-      <c r="EM15"/>
-      <c r="EN15"/>
-      <c r="EO15"/>
-      <c r="EP15"/>
-      <c r="EQ15"/>
-      <c r="ER15"/>
-      <c r="ES15"/>
-      <c r="ET15"/>
-      <c r="EU15"/>
-      <c r="EV15"/>
-      <c r="EW15"/>
-      <c r="EX15"/>
-      <c r="EY15"/>
-      <c r="EZ15"/>
-      <c r="FA15"/>
-      <c r="FB15"/>
-      <c r="FC15"/>
-    </row>
-    <row r="16" spans="1:159" s="3" customFormat="1">
+    </row>
+    <row r="16" spans="1:28" s="3" customFormat="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -4564,139 +4042,8 @@
       <c r="Z16"/>
       <c r="AA16"/>
       <c r="AB16"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
-      <c r="AE16"/>
-      <c r="AF16"/>
-      <c r="AG16"/>
-      <c r="AH16"/>
-      <c r="AI16"/>
-      <c r="AJ16"/>
-      <c r="AK16"/>
-      <c r="AL16"/>
-      <c r="AM16"/>
-      <c r="AN16"/>
-      <c r="AO16"/>
-      <c r="AP16"/>
-      <c r="AQ16"/>
-      <c r="AR16"/>
-      <c r="AS16"/>
-      <c r="AT16"/>
-      <c r="AU16"/>
-      <c r="AV16"/>
-      <c r="AW16"/>
-      <c r="AX16"/>
-      <c r="AY16"/>
-      <c r="AZ16"/>
-      <c r="BA16"/>
-      <c r="BB16"/>
-      <c r="BC16"/>
-      <c r="BD16"/>
-      <c r="BE16"/>
-      <c r="BF16"/>
-      <c r="BG16"/>
-      <c r="BH16"/>
-      <c r="BI16"/>
-      <c r="BJ16"/>
-      <c r="BK16"/>
-      <c r="BL16"/>
-      <c r="BM16"/>
-      <c r="BN16"/>
-      <c r="BO16"/>
-      <c r="BP16"/>
-      <c r="BQ16"/>
-      <c r="BR16"/>
-      <c r="BS16"/>
-      <c r="BT16"/>
-      <c r="BU16"/>
-      <c r="BV16"/>
-      <c r="BW16"/>
-      <c r="BX16"/>
-      <c r="BY16"/>
-      <c r="BZ16"/>
-      <c r="CA16"/>
-      <c r="CB16"/>
-      <c r="CC16"/>
-      <c r="CD16"/>
-      <c r="CE16"/>
-      <c r="CF16"/>
-      <c r="CG16"/>
-      <c r="CH16"/>
-      <c r="CI16"/>
-      <c r="CJ16"/>
-      <c r="CK16"/>
-      <c r="CL16"/>
-      <c r="CM16"/>
-      <c r="CN16"/>
-      <c r="CO16"/>
-      <c r="CP16"/>
-      <c r="CQ16"/>
-      <c r="CR16"/>
-      <c r="CS16"/>
-      <c r="CT16"/>
-      <c r="CU16"/>
-      <c r="CV16"/>
-      <c r="CW16"/>
-      <c r="CX16"/>
-      <c r="CY16"/>
-      <c r="CZ16"/>
-      <c r="DA16"/>
-      <c r="DB16"/>
-      <c r="DC16"/>
-      <c r="DD16"/>
-      <c r="DE16"/>
-      <c r="DF16"/>
-      <c r="DG16"/>
-      <c r="DH16"/>
-      <c r="DI16"/>
-      <c r="DJ16"/>
-      <c r="DK16"/>
-      <c r="DL16"/>
-      <c r="DM16"/>
-      <c r="DN16"/>
-      <c r="DO16"/>
-      <c r="DP16"/>
-      <c r="DQ16"/>
-      <c r="DR16"/>
-      <c r="DS16"/>
-      <c r="DT16"/>
-      <c r="DU16"/>
-      <c r="DV16"/>
-      <c r="DW16"/>
-      <c r="DX16"/>
-      <c r="DY16"/>
-      <c r="DZ16"/>
-      <c r="EA16"/>
-      <c r="EB16"/>
-      <c r="EC16"/>
-      <c r="ED16"/>
-      <c r="EE16"/>
-      <c r="EF16"/>
-      <c r="EG16"/>
-      <c r="EH16"/>
-      <c r="EI16"/>
-      <c r="EJ16"/>
-      <c r="EK16"/>
-      <c r="EL16"/>
-      <c r="EM16"/>
-      <c r="EN16"/>
-      <c r="EO16"/>
-      <c r="EP16"/>
-      <c r="EQ16"/>
-      <c r="ER16"/>
-      <c r="ES16"/>
-      <c r="ET16"/>
-      <c r="EU16"/>
-      <c r="EV16"/>
-      <c r="EW16"/>
-      <c r="EX16"/>
-      <c r="EY16"/>
-      <c r="EZ16"/>
-      <c r="FA16"/>
-      <c r="FB16"/>
-      <c r="FC16"/>
-    </row>
-    <row r="17" spans="1:159" s="3" customFormat="1">
+    </row>
+    <row r="17" spans="1:28" s="3" customFormat="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -4754,139 +4101,8 @@
       <c r="Z17"/>
       <c r="AA17"/>
       <c r="AB17"/>
-      <c r="AC17"/>
-      <c r="AD17"/>
-      <c r="AE17"/>
-      <c r="AF17"/>
-      <c r="AG17"/>
-      <c r="AH17"/>
-      <c r="AI17"/>
-      <c r="AJ17"/>
-      <c r="AK17"/>
-      <c r="AL17"/>
-      <c r="AM17"/>
-      <c r="AN17"/>
-      <c r="AO17"/>
-      <c r="AP17"/>
-      <c r="AQ17"/>
-      <c r="AR17"/>
-      <c r="AS17"/>
-      <c r="AT17"/>
-      <c r="AU17"/>
-      <c r="AV17"/>
-      <c r="AW17"/>
-      <c r="AX17"/>
-      <c r="AY17"/>
-      <c r="AZ17"/>
-      <c r="BA17"/>
-      <c r="BB17"/>
-      <c r="BC17"/>
-      <c r="BD17"/>
-      <c r="BE17"/>
-      <c r="BF17"/>
-      <c r="BG17"/>
-      <c r="BH17"/>
-      <c r="BI17"/>
-      <c r="BJ17"/>
-      <c r="BK17"/>
-      <c r="BL17"/>
-      <c r="BM17"/>
-      <c r="BN17"/>
-      <c r="BO17"/>
-      <c r="BP17"/>
-      <c r="BQ17"/>
-      <c r="BR17"/>
-      <c r="BS17"/>
-      <c r="BT17"/>
-      <c r="BU17"/>
-      <c r="BV17"/>
-      <c r="BW17"/>
-      <c r="BX17"/>
-      <c r="BY17"/>
-      <c r="BZ17"/>
-      <c r="CA17"/>
-      <c r="CB17"/>
-      <c r="CC17"/>
-      <c r="CD17"/>
-      <c r="CE17"/>
-      <c r="CF17"/>
-      <c r="CG17"/>
-      <c r="CH17"/>
-      <c r="CI17"/>
-      <c r="CJ17"/>
-      <c r="CK17"/>
-      <c r="CL17"/>
-      <c r="CM17"/>
-      <c r="CN17"/>
-      <c r="CO17"/>
-      <c r="CP17"/>
-      <c r="CQ17"/>
-      <c r="CR17"/>
-      <c r="CS17"/>
-      <c r="CT17"/>
-      <c r="CU17"/>
-      <c r="CV17"/>
-      <c r="CW17"/>
-      <c r="CX17"/>
-      <c r="CY17"/>
-      <c r="CZ17"/>
-      <c r="DA17"/>
-      <c r="DB17"/>
-      <c r="DC17"/>
-      <c r="DD17"/>
-      <c r="DE17"/>
-      <c r="DF17"/>
-      <c r="DG17"/>
-      <c r="DH17"/>
-      <c r="DI17"/>
-      <c r="DJ17"/>
-      <c r="DK17"/>
-      <c r="DL17"/>
-      <c r="DM17"/>
-      <c r="DN17"/>
-      <c r="DO17"/>
-      <c r="DP17"/>
-      <c r="DQ17"/>
-      <c r="DR17"/>
-      <c r="DS17"/>
-      <c r="DT17"/>
-      <c r="DU17"/>
-      <c r="DV17"/>
-      <c r="DW17"/>
-      <c r="DX17"/>
-      <c r="DY17"/>
-      <c r="DZ17"/>
-      <c r="EA17"/>
-      <c r="EB17"/>
-      <c r="EC17"/>
-      <c r="ED17"/>
-      <c r="EE17"/>
-      <c r="EF17"/>
-      <c r="EG17"/>
-      <c r="EH17"/>
-      <c r="EI17"/>
-      <c r="EJ17"/>
-      <c r="EK17"/>
-      <c r="EL17"/>
-      <c r="EM17"/>
-      <c r="EN17"/>
-      <c r="EO17"/>
-      <c r="EP17"/>
-      <c r="EQ17"/>
-      <c r="ER17"/>
-      <c r="ES17"/>
-      <c r="ET17"/>
-      <c r="EU17"/>
-      <c r="EV17"/>
-      <c r="EW17"/>
-      <c r="EX17"/>
-      <c r="EY17"/>
-      <c r="EZ17"/>
-      <c r="FA17"/>
-      <c r="FB17"/>
-      <c r="FC17"/>
-    </row>
-    <row r="18" spans="1:159">
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4931,7 +4147,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="19" spans="1:159">
+    <row r="19" spans="1:28">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4976,7 +4192,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:159">
+    <row r="20" spans="1:28">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5021,7 +4237,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:159">
+    <row r="21" spans="1:28">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5066,7 +4282,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:159">
+    <row r="22" spans="1:28">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5111,7 +4327,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:159">
+    <row r="23" spans="1:28">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5156,7 +4372,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:159">
+    <row r="24" spans="1:28">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5201,7 +4417,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:159">
+    <row r="25" spans="1:28">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5246,7 +4462,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="26" spans="1:159">
+    <row r="26" spans="1:28">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5291,7 +4507,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="1:159">
+    <row r="27" spans="1:28">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -5344,8 +4560,14 @@
       <c r="V27" s="31">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="28" spans="1:159">
+      <c r="Z27" s="56">
+        <v>41.4</v>
+      </c>
+      <c r="AA27" s="60">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -5398,8 +4620,14 @@
       <c r="V28" s="32">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="29" spans="1:159">
+      <c r="Z28" s="57">
+        <v>24.3</v>
+      </c>
+      <c r="AA28" s="61">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -5452,8 +4680,14 @@
       <c r="V29" s="32">
         <v>2.65</v>
       </c>
-    </row>
-    <row r="30" spans="1:159">
+      <c r="Z29" s="57">
+        <v>23.2</v>
+      </c>
+      <c r="AA29" s="61">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -5506,8 +4740,14 @@
       <c r="V30" s="32">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:159">
+      <c r="Z30" s="57">
+        <v>25.6</v>
+      </c>
+      <c r="AA30" s="61">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -5560,8 +4800,14 @@
       <c r="V31" s="32">
         <v>3.35</v>
       </c>
-    </row>
-    <row r="32" spans="1:159">
+      <c r="Z31" s="57">
+        <v>31.1</v>
+      </c>
+      <c r="AA31" s="61">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -5614,8 +4860,14 @@
       <c r="V32" s="32">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="33" spans="1:159" s="3" customFormat="1">
+      <c r="Z32" s="57">
+        <v>34.5</v>
+      </c>
+      <c r="AA32" s="61">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" s="3" customFormat="1">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -5676,142 +4928,15 @@
       <c r="W33"/>
       <c r="X33"/>
       <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
+      <c r="Z33" s="57">
+        <v>39.4</v>
+      </c>
+      <c r="AA33" s="61">
+        <v>3.9</v>
+      </c>
       <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-      <c r="AR33"/>
-      <c r="AS33"/>
-      <c r="AT33"/>
-      <c r="AU33"/>
-      <c r="AV33"/>
-      <c r="AW33"/>
-      <c r="AX33"/>
-      <c r="AY33"/>
-      <c r="AZ33"/>
-      <c r="BA33"/>
-      <c r="BB33"/>
-      <c r="BC33"/>
-      <c r="BD33"/>
-      <c r="BE33"/>
-      <c r="BF33"/>
-      <c r="BG33"/>
-      <c r="BH33"/>
-      <c r="BI33"/>
-      <c r="BJ33"/>
-      <c r="BK33"/>
-      <c r="BL33"/>
-      <c r="BM33"/>
-      <c r="BN33"/>
-      <c r="BO33"/>
-      <c r="BP33"/>
-      <c r="BQ33"/>
-      <c r="BR33"/>
-      <c r="BS33"/>
-      <c r="BT33"/>
-      <c r="BU33"/>
-      <c r="BV33"/>
-      <c r="BW33"/>
-      <c r="BX33"/>
-      <c r="BY33"/>
-      <c r="BZ33"/>
-      <c r="CA33"/>
-      <c r="CB33"/>
-      <c r="CC33"/>
-      <c r="CD33"/>
-      <c r="CE33"/>
-      <c r="CF33"/>
-      <c r="CG33"/>
-      <c r="CH33"/>
-      <c r="CI33"/>
-      <c r="CJ33"/>
-      <c r="CK33"/>
-      <c r="CL33"/>
-      <c r="CM33"/>
-      <c r="CN33"/>
-      <c r="CO33"/>
-      <c r="CP33"/>
-      <c r="CQ33"/>
-      <c r="CR33"/>
-      <c r="CS33"/>
-      <c r="CT33"/>
-      <c r="CU33"/>
-      <c r="CV33"/>
-      <c r="CW33"/>
-      <c r="CX33"/>
-      <c r="CY33"/>
-      <c r="CZ33"/>
-      <c r="DA33"/>
-      <c r="DB33"/>
-      <c r="DC33"/>
-      <c r="DD33"/>
-      <c r="DE33"/>
-      <c r="DF33"/>
-      <c r="DG33"/>
-      <c r="DH33"/>
-      <c r="DI33"/>
-      <c r="DJ33"/>
-      <c r="DK33"/>
-      <c r="DL33"/>
-      <c r="DM33"/>
-      <c r="DN33"/>
-      <c r="DO33"/>
-      <c r="DP33"/>
-      <c r="DQ33"/>
-      <c r="DR33"/>
-      <c r="DS33"/>
-      <c r="DT33"/>
-      <c r="DU33"/>
-      <c r="DV33"/>
-      <c r="DW33"/>
-      <c r="DX33"/>
-      <c r="DY33"/>
-      <c r="DZ33"/>
-      <c r="EA33"/>
-      <c r="EB33"/>
-      <c r="EC33"/>
-      <c r="ED33"/>
-      <c r="EE33"/>
-      <c r="EF33"/>
-      <c r="EG33"/>
-      <c r="EH33"/>
-      <c r="EI33"/>
-      <c r="EJ33"/>
-      <c r="EK33"/>
-      <c r="EL33"/>
-      <c r="EM33"/>
-      <c r="EN33"/>
-      <c r="EO33"/>
-      <c r="EP33"/>
-      <c r="EQ33"/>
-      <c r="ER33"/>
-      <c r="ES33"/>
-      <c r="ET33"/>
-      <c r="EU33"/>
-      <c r="EV33"/>
-      <c r="EW33"/>
-      <c r="EX33"/>
-      <c r="EY33"/>
-      <c r="EZ33"/>
-      <c r="FA33"/>
-      <c r="FB33"/>
-      <c r="FC33"/>
-    </row>
-    <row r="34" spans="1:159" s="3" customFormat="1" ht="15" thickBot="1">
+    </row>
+    <row r="34" spans="1:28" s="3" customFormat="1" ht="15" thickBot="1">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -5872,142 +4997,15 @@
       <c r="W34"/>
       <c r="X34"/>
       <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
+      <c r="Z34" s="58">
+        <v>69</v>
+      </c>
+      <c r="AA34" s="62">
+        <v>3.9</v>
+      </c>
       <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-      <c r="AR34"/>
-      <c r="AS34"/>
-      <c r="AT34"/>
-      <c r="AU34"/>
-      <c r="AV34"/>
-      <c r="AW34"/>
-      <c r="AX34"/>
-      <c r="AY34"/>
-      <c r="AZ34"/>
-      <c r="BA34"/>
-      <c r="BB34"/>
-      <c r="BC34"/>
-      <c r="BD34"/>
-      <c r="BE34"/>
-      <c r="BF34"/>
-      <c r="BG34"/>
-      <c r="BH34"/>
-      <c r="BI34"/>
-      <c r="BJ34"/>
-      <c r="BK34"/>
-      <c r="BL34"/>
-      <c r="BM34"/>
-      <c r="BN34"/>
-      <c r="BO34"/>
-      <c r="BP34"/>
-      <c r="BQ34"/>
-      <c r="BR34"/>
-      <c r="BS34"/>
-      <c r="BT34"/>
-      <c r="BU34"/>
-      <c r="BV34"/>
-      <c r="BW34"/>
-      <c r="BX34"/>
-      <c r="BY34"/>
-      <c r="BZ34"/>
-      <c r="CA34"/>
-      <c r="CB34"/>
-      <c r="CC34"/>
-      <c r="CD34"/>
-      <c r="CE34"/>
-      <c r="CF34"/>
-      <c r="CG34"/>
-      <c r="CH34"/>
-      <c r="CI34"/>
-      <c r="CJ34"/>
-      <c r="CK34"/>
-      <c r="CL34"/>
-      <c r="CM34"/>
-      <c r="CN34"/>
-      <c r="CO34"/>
-      <c r="CP34"/>
-      <c r="CQ34"/>
-      <c r="CR34"/>
-      <c r="CS34"/>
-      <c r="CT34"/>
-      <c r="CU34"/>
-      <c r="CV34"/>
-      <c r="CW34"/>
-      <c r="CX34"/>
-      <c r="CY34"/>
-      <c r="CZ34"/>
-      <c r="DA34"/>
-      <c r="DB34"/>
-      <c r="DC34"/>
-      <c r="DD34"/>
-      <c r="DE34"/>
-      <c r="DF34"/>
-      <c r="DG34"/>
-      <c r="DH34"/>
-      <c r="DI34"/>
-      <c r="DJ34"/>
-      <c r="DK34"/>
-      <c r="DL34"/>
-      <c r="DM34"/>
-      <c r="DN34"/>
-      <c r="DO34"/>
-      <c r="DP34"/>
-      <c r="DQ34"/>
-      <c r="DR34"/>
-      <c r="DS34"/>
-      <c r="DT34"/>
-      <c r="DU34"/>
-      <c r="DV34"/>
-      <c r="DW34"/>
-      <c r="DX34"/>
-      <c r="DY34"/>
-      <c r="DZ34"/>
-      <c r="EA34"/>
-      <c r="EB34"/>
-      <c r="EC34"/>
-      <c r="ED34"/>
-      <c r="EE34"/>
-      <c r="EF34"/>
-      <c r="EG34"/>
-      <c r="EH34"/>
-      <c r="EI34"/>
-      <c r="EJ34"/>
-      <c r="EK34"/>
-      <c r="EL34"/>
-      <c r="EM34"/>
-      <c r="EN34"/>
-      <c r="EO34"/>
-      <c r="EP34"/>
-      <c r="EQ34"/>
-      <c r="ER34"/>
-      <c r="ES34"/>
-      <c r="ET34"/>
-      <c r="EU34"/>
-      <c r="EV34"/>
-      <c r="EW34"/>
-      <c r="EX34"/>
-      <c r="EY34"/>
-      <c r="EZ34"/>
-      <c r="FA34"/>
-      <c r="FB34"/>
-      <c r="FC34"/>
-    </row>
-    <row r="35" spans="1:159" s="3" customFormat="1" ht="15" thickTop="1">
+    </row>
+    <row r="35" spans="1:28" s="3" customFormat="1" ht="15" thickTop="1">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6068,142 +5066,15 @@
       <c r="W35"/>
       <c r="X35"/>
       <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
+      <c r="Z35" s="56">
+        <v>17.88</v>
+      </c>
+      <c r="AA35" s="60">
+        <v>0.30000000000000004</v>
+      </c>
       <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-      <c r="AR35"/>
-      <c r="AS35"/>
-      <c r="AT35"/>
-      <c r="AU35"/>
-      <c r="AV35"/>
-      <c r="AW35"/>
-      <c r="AX35"/>
-      <c r="AY35"/>
-      <c r="AZ35"/>
-      <c r="BA35"/>
-      <c r="BB35"/>
-      <c r="BC35"/>
-      <c r="BD35"/>
-      <c r="BE35"/>
-      <c r="BF35"/>
-      <c r="BG35"/>
-      <c r="BH35"/>
-      <c r="BI35"/>
-      <c r="BJ35"/>
-      <c r="BK35"/>
-      <c r="BL35"/>
-      <c r="BM35"/>
-      <c r="BN35"/>
-      <c r="BO35"/>
-      <c r="BP35"/>
-      <c r="BQ35"/>
-      <c r="BR35"/>
-      <c r="BS35"/>
-      <c r="BT35"/>
-      <c r="BU35"/>
-      <c r="BV35"/>
-      <c r="BW35"/>
-      <c r="BX35"/>
-      <c r="BY35"/>
-      <c r="BZ35"/>
-      <c r="CA35"/>
-      <c r="CB35"/>
-      <c r="CC35"/>
-      <c r="CD35"/>
-      <c r="CE35"/>
-      <c r="CF35"/>
-      <c r="CG35"/>
-      <c r="CH35"/>
-      <c r="CI35"/>
-      <c r="CJ35"/>
-      <c r="CK35"/>
-      <c r="CL35"/>
-      <c r="CM35"/>
-      <c r="CN35"/>
-      <c r="CO35"/>
-      <c r="CP35"/>
-      <c r="CQ35"/>
-      <c r="CR35"/>
-      <c r="CS35"/>
-      <c r="CT35"/>
-      <c r="CU35"/>
-      <c r="CV35"/>
-      <c r="CW35"/>
-      <c r="CX35"/>
-      <c r="CY35"/>
-      <c r="CZ35"/>
-      <c r="DA35"/>
-      <c r="DB35"/>
-      <c r="DC35"/>
-      <c r="DD35"/>
-      <c r="DE35"/>
-      <c r="DF35"/>
-      <c r="DG35"/>
-      <c r="DH35"/>
-      <c r="DI35"/>
-      <c r="DJ35"/>
-      <c r="DK35"/>
-      <c r="DL35"/>
-      <c r="DM35"/>
-      <c r="DN35"/>
-      <c r="DO35"/>
-      <c r="DP35"/>
-      <c r="DQ35"/>
-      <c r="DR35"/>
-      <c r="DS35"/>
-      <c r="DT35"/>
-      <c r="DU35"/>
-      <c r="DV35"/>
-      <c r="DW35"/>
-      <c r="DX35"/>
-      <c r="DY35"/>
-      <c r="DZ35"/>
-      <c r="EA35"/>
-      <c r="EB35"/>
-      <c r="EC35"/>
-      <c r="ED35"/>
-      <c r="EE35"/>
-      <c r="EF35"/>
-      <c r="EG35"/>
-      <c r="EH35"/>
-      <c r="EI35"/>
-      <c r="EJ35"/>
-      <c r="EK35"/>
-      <c r="EL35"/>
-      <c r="EM35"/>
-      <c r="EN35"/>
-      <c r="EO35"/>
-      <c r="EP35"/>
-      <c r="EQ35"/>
-      <c r="ER35"/>
-      <c r="ES35"/>
-      <c r="ET35"/>
-      <c r="EU35"/>
-      <c r="EV35"/>
-      <c r="EW35"/>
-      <c r="EX35"/>
-      <c r="EY35"/>
-      <c r="EZ35"/>
-      <c r="FA35"/>
-      <c r="FB35"/>
-      <c r="FC35"/>
-    </row>
-    <row r="36" spans="1:159">
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6256,8 +5127,14 @@
       <c r="V36" s="32">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:159">
+      <c r="Z36" s="57">
+        <v>18.63</v>
+      </c>
+      <c r="AA36" s="61">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -6310,8 +5187,14 @@
       <c r="V37" s="32">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:159">
+      <c r="Z37" s="57">
+        <v>18.72</v>
+      </c>
+      <c r="AA37" s="61">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -6364,8 +5247,14 @@
       <c r="V38" s="32">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:159">
+      <c r="Z38" s="57">
+        <v>20.57</v>
+      </c>
+      <c r="AA38" s="61">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -6418,8 +5307,14 @@
       <c r="V39" s="32">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:159">
+      <c r="Z39" s="57">
+        <v>20.36</v>
+      </c>
+      <c r="AA39" s="61">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -6472,8 +5367,14 @@
       <c r="V40" s="32">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:159">
+      <c r="Z40" s="57">
+        <v>20.16</v>
+      </c>
+      <c r="AA40" s="61">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -6526,8 +5427,14 @@
       <c r="V41" s="32">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:159" ht="15" thickBot="1">
+      <c r="Z41" s="57">
+        <v>56.5</v>
+      </c>
+      <c r="AA41" s="61">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="15" thickBot="1">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -6580,8 +5487,14 @@
       <c r="V42" s="33">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:159" ht="15" thickTop="1">
+      <c r="Z42" s="58">
+        <v>60.3</v>
+      </c>
+      <c r="AA42" s="62">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="15" thickTop="1">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -6634,8 +5547,14 @@
       <c r="V43" s="34">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="44" spans="1:159">
+      <c r="Z43" s="56">
+        <v>69</v>
+      </c>
+      <c r="AA43" s="60">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -6688,8 +5607,14 @@
       <c r="V44" s="32">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:159">
+      <c r="Z44" s="57">
+        <v>69</v>
+      </c>
+      <c r="AA44" s="61">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -6742,8 +5667,14 @@
       <c r="V45" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:159" s="3" customFormat="1">
+      <c r="Z45" s="57">
+        <v>72.2</v>
+      </c>
+      <c r="AA45" s="61">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" s="3" customFormat="1">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -6804,142 +5735,15 @@
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
-      <c r="Z46"/>
-      <c r="AA46"/>
+      <c r="Z46" s="57">
+        <v>81.5</v>
+      </c>
+      <c r="AA46" s="61">
+        <v>1.9</v>
+      </c>
       <c r="AB46"/>
-      <c r="AC46"/>
-      <c r="AD46"/>
-      <c r="AE46"/>
-      <c r="AF46"/>
-      <c r="AG46"/>
-      <c r="AH46"/>
-      <c r="AI46"/>
-      <c r="AJ46"/>
-      <c r="AK46"/>
-      <c r="AL46"/>
-      <c r="AM46"/>
-      <c r="AN46"/>
-      <c r="AO46"/>
-      <c r="AP46"/>
-      <c r="AQ46"/>
-      <c r="AR46"/>
-      <c r="AS46"/>
-      <c r="AT46"/>
-      <c r="AU46"/>
-      <c r="AV46"/>
-      <c r="AW46"/>
-      <c r="AX46"/>
-      <c r="AY46"/>
-      <c r="AZ46"/>
-      <c r="BA46"/>
-      <c r="BB46"/>
-      <c r="BC46"/>
-      <c r="BD46"/>
-      <c r="BE46"/>
-      <c r="BF46"/>
-      <c r="BG46"/>
-      <c r="BH46"/>
-      <c r="BI46"/>
-      <c r="BJ46"/>
-      <c r="BK46"/>
-      <c r="BL46"/>
-      <c r="BM46"/>
-      <c r="BN46"/>
-      <c r="BO46"/>
-      <c r="BP46"/>
-      <c r="BQ46"/>
-      <c r="BR46"/>
-      <c r="BS46"/>
-      <c r="BT46"/>
-      <c r="BU46"/>
-      <c r="BV46"/>
-      <c r="BW46"/>
-      <c r="BX46"/>
-      <c r="BY46"/>
-      <c r="BZ46"/>
-      <c r="CA46"/>
-      <c r="CB46"/>
-      <c r="CC46"/>
-      <c r="CD46"/>
-      <c r="CE46"/>
-      <c r="CF46"/>
-      <c r="CG46"/>
-      <c r="CH46"/>
-      <c r="CI46"/>
-      <c r="CJ46"/>
-      <c r="CK46"/>
-      <c r="CL46"/>
-      <c r="CM46"/>
-      <c r="CN46"/>
-      <c r="CO46"/>
-      <c r="CP46"/>
-      <c r="CQ46"/>
-      <c r="CR46"/>
-      <c r="CS46"/>
-      <c r="CT46"/>
-      <c r="CU46"/>
-      <c r="CV46"/>
-      <c r="CW46"/>
-      <c r="CX46"/>
-      <c r="CY46"/>
-      <c r="CZ46"/>
-      <c r="DA46"/>
-      <c r="DB46"/>
-      <c r="DC46"/>
-      <c r="DD46"/>
-      <c r="DE46"/>
-      <c r="DF46"/>
-      <c r="DG46"/>
-      <c r="DH46"/>
-      <c r="DI46"/>
-      <c r="DJ46"/>
-      <c r="DK46"/>
-      <c r="DL46"/>
-      <c r="DM46"/>
-      <c r="DN46"/>
-      <c r="DO46"/>
-      <c r="DP46"/>
-      <c r="DQ46"/>
-      <c r="DR46"/>
-      <c r="DS46"/>
-      <c r="DT46"/>
-      <c r="DU46"/>
-      <c r="DV46"/>
-      <c r="DW46"/>
-      <c r="DX46"/>
-      <c r="DY46"/>
-      <c r="DZ46"/>
-      <c r="EA46"/>
-      <c r="EB46"/>
-      <c r="EC46"/>
-      <c r="ED46"/>
-      <c r="EE46"/>
-      <c r="EF46"/>
-      <c r="EG46"/>
-      <c r="EH46"/>
-      <c r="EI46"/>
-      <c r="EJ46"/>
-      <c r="EK46"/>
-      <c r="EL46"/>
-      <c r="EM46"/>
-      <c r="EN46"/>
-      <c r="EO46"/>
-      <c r="EP46"/>
-      <c r="EQ46"/>
-      <c r="ER46"/>
-      <c r="ES46"/>
-      <c r="ET46"/>
-      <c r="EU46"/>
-      <c r="EV46"/>
-      <c r="EW46"/>
-      <c r="EX46"/>
-      <c r="EY46"/>
-      <c r="EZ46"/>
-      <c r="FA46"/>
-      <c r="FB46"/>
-      <c r="FC46"/>
-    </row>
-    <row r="47" spans="1:159" s="3" customFormat="1">
+    </row>
+    <row r="47" spans="1:28" s="3" customFormat="1">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7000,142 +5804,15 @@
       <c r="W47"/>
       <c r="X47"/>
       <c r="Y47"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
+      <c r="Z47" s="57">
+        <v>84.5</v>
+      </c>
+      <c r="AA47" s="61">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="AB47"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
-      <c r="AE47"/>
-      <c r="AF47"/>
-      <c r="AG47"/>
-      <c r="AH47"/>
-      <c r="AI47"/>
-      <c r="AJ47"/>
-      <c r="AK47"/>
-      <c r="AL47"/>
-      <c r="AM47"/>
-      <c r="AN47"/>
-      <c r="AO47"/>
-      <c r="AP47"/>
-      <c r="AQ47"/>
-      <c r="AR47"/>
-      <c r="AS47"/>
-      <c r="AT47"/>
-      <c r="AU47"/>
-      <c r="AV47"/>
-      <c r="AW47"/>
-      <c r="AX47"/>
-      <c r="AY47"/>
-      <c r="AZ47"/>
-      <c r="BA47"/>
-      <c r="BB47"/>
-      <c r="BC47"/>
-      <c r="BD47"/>
-      <c r="BE47"/>
-      <c r="BF47"/>
-      <c r="BG47"/>
-      <c r="BH47"/>
-      <c r="BI47"/>
-      <c r="BJ47"/>
-      <c r="BK47"/>
-      <c r="BL47"/>
-      <c r="BM47"/>
-      <c r="BN47"/>
-      <c r="BO47"/>
-      <c r="BP47"/>
-      <c r="BQ47"/>
-      <c r="BR47"/>
-      <c r="BS47"/>
-      <c r="BT47"/>
-      <c r="BU47"/>
-      <c r="BV47"/>
-      <c r="BW47"/>
-      <c r="BX47"/>
-      <c r="BY47"/>
-      <c r="BZ47"/>
-      <c r="CA47"/>
-      <c r="CB47"/>
-      <c r="CC47"/>
-      <c r="CD47"/>
-      <c r="CE47"/>
-      <c r="CF47"/>
-      <c r="CG47"/>
-      <c r="CH47"/>
-      <c r="CI47"/>
-      <c r="CJ47"/>
-      <c r="CK47"/>
-      <c r="CL47"/>
-      <c r="CM47"/>
-      <c r="CN47"/>
-      <c r="CO47"/>
-      <c r="CP47"/>
-      <c r="CQ47"/>
-      <c r="CR47"/>
-      <c r="CS47"/>
-      <c r="CT47"/>
-      <c r="CU47"/>
-      <c r="CV47"/>
-      <c r="CW47"/>
-      <c r="CX47"/>
-      <c r="CY47"/>
-      <c r="CZ47"/>
-      <c r="DA47"/>
-      <c r="DB47"/>
-      <c r="DC47"/>
-      <c r="DD47"/>
-      <c r="DE47"/>
-      <c r="DF47"/>
-      <c r="DG47"/>
-      <c r="DH47"/>
-      <c r="DI47"/>
-      <c r="DJ47"/>
-      <c r="DK47"/>
-      <c r="DL47"/>
-      <c r="DM47"/>
-      <c r="DN47"/>
-      <c r="DO47"/>
-      <c r="DP47"/>
-      <c r="DQ47"/>
-      <c r="DR47"/>
-      <c r="DS47"/>
-      <c r="DT47"/>
-      <c r="DU47"/>
-      <c r="DV47"/>
-      <c r="DW47"/>
-      <c r="DX47"/>
-      <c r="DY47"/>
-      <c r="DZ47"/>
-      <c r="EA47"/>
-      <c r="EB47"/>
-      <c r="EC47"/>
-      <c r="ED47"/>
-      <c r="EE47"/>
-      <c r="EF47"/>
-      <c r="EG47"/>
-      <c r="EH47"/>
-      <c r="EI47"/>
-      <c r="EJ47"/>
-      <c r="EK47"/>
-      <c r="EL47"/>
-      <c r="EM47"/>
-      <c r="EN47"/>
-      <c r="EO47"/>
-      <c r="EP47"/>
-      <c r="EQ47"/>
-      <c r="ER47"/>
-      <c r="ES47"/>
-      <c r="ET47"/>
-      <c r="EU47"/>
-      <c r="EV47"/>
-      <c r="EW47"/>
-      <c r="EX47"/>
-      <c r="EY47"/>
-      <c r="EZ47"/>
-      <c r="FA47"/>
-      <c r="FB47"/>
-      <c r="FC47"/>
-    </row>
-    <row r="48" spans="1:159" s="3" customFormat="1">
+    </row>
+    <row r="48" spans="1:28" s="3" customFormat="1">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7196,142 +5873,15 @@
       <c r="W48"/>
       <c r="X48"/>
       <c r="Y48"/>
-      <c r="Z48"/>
-      <c r="AA48"/>
+      <c r="Z48" s="57">
+        <v>103</v>
+      </c>
+      <c r="AA48" s="61">
+        <v>3</v>
+      </c>
       <c r="AB48"/>
-      <c r="AC48"/>
-      <c r="AD48"/>
-      <c r="AE48"/>
-      <c r="AF48"/>
-      <c r="AG48"/>
-      <c r="AH48"/>
-      <c r="AI48"/>
-      <c r="AJ48"/>
-      <c r="AK48"/>
-      <c r="AL48"/>
-      <c r="AM48"/>
-      <c r="AN48"/>
-      <c r="AO48"/>
-      <c r="AP48"/>
-      <c r="AQ48"/>
-      <c r="AR48"/>
-      <c r="AS48"/>
-      <c r="AT48"/>
-      <c r="AU48"/>
-      <c r="AV48"/>
-      <c r="AW48"/>
-      <c r="AX48"/>
-      <c r="AY48"/>
-      <c r="AZ48"/>
-      <c r="BA48"/>
-      <c r="BB48"/>
-      <c r="BC48"/>
-      <c r="BD48"/>
-      <c r="BE48"/>
-      <c r="BF48"/>
-      <c r="BG48"/>
-      <c r="BH48"/>
-      <c r="BI48"/>
-      <c r="BJ48"/>
-      <c r="BK48"/>
-      <c r="BL48"/>
-      <c r="BM48"/>
-      <c r="BN48"/>
-      <c r="BO48"/>
-      <c r="BP48"/>
-      <c r="BQ48"/>
-      <c r="BR48"/>
-      <c r="BS48"/>
-      <c r="BT48"/>
-      <c r="BU48"/>
-      <c r="BV48"/>
-      <c r="BW48"/>
-      <c r="BX48"/>
-      <c r="BY48"/>
-      <c r="BZ48"/>
-      <c r="CA48"/>
-      <c r="CB48"/>
-      <c r="CC48"/>
-      <c r="CD48"/>
-      <c r="CE48"/>
-      <c r="CF48"/>
-      <c r="CG48"/>
-      <c r="CH48"/>
-      <c r="CI48"/>
-      <c r="CJ48"/>
-      <c r="CK48"/>
-      <c r="CL48"/>
-      <c r="CM48"/>
-      <c r="CN48"/>
-      <c r="CO48"/>
-      <c r="CP48"/>
-      <c r="CQ48"/>
-      <c r="CR48"/>
-      <c r="CS48"/>
-      <c r="CT48"/>
-      <c r="CU48"/>
-      <c r="CV48"/>
-      <c r="CW48"/>
-      <c r="CX48"/>
-      <c r="CY48"/>
-      <c r="CZ48"/>
-      <c r="DA48"/>
-      <c r="DB48"/>
-      <c r="DC48"/>
-      <c r="DD48"/>
-      <c r="DE48"/>
-      <c r="DF48"/>
-      <c r="DG48"/>
-      <c r="DH48"/>
-      <c r="DI48"/>
-      <c r="DJ48"/>
-      <c r="DK48"/>
-      <c r="DL48"/>
-      <c r="DM48"/>
-      <c r="DN48"/>
-      <c r="DO48"/>
-      <c r="DP48"/>
-      <c r="DQ48"/>
-      <c r="DR48"/>
-      <c r="DS48"/>
-      <c r="DT48"/>
-      <c r="DU48"/>
-      <c r="DV48"/>
-      <c r="DW48"/>
-      <c r="DX48"/>
-      <c r="DY48"/>
-      <c r="DZ48"/>
-      <c r="EA48"/>
-      <c r="EB48"/>
-      <c r="EC48"/>
-      <c r="ED48"/>
-      <c r="EE48"/>
-      <c r="EF48"/>
-      <c r="EG48"/>
-      <c r="EH48"/>
-      <c r="EI48"/>
-      <c r="EJ48"/>
-      <c r="EK48"/>
-      <c r="EL48"/>
-      <c r="EM48"/>
-      <c r="EN48"/>
-      <c r="EO48"/>
-      <c r="EP48"/>
-      <c r="EQ48"/>
-      <c r="ER48"/>
-      <c r="ES48"/>
-      <c r="ET48"/>
-      <c r="EU48"/>
-      <c r="EV48"/>
-      <c r="EW48"/>
-      <c r="EX48"/>
-      <c r="EY48"/>
-      <c r="EZ48"/>
-      <c r="FA48"/>
-      <c r="FB48"/>
-      <c r="FC48"/>
-    </row>
-    <row r="49" spans="1:22">
+    </row>
+    <row r="49" spans="1:27">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -7384,8 +5934,14 @@
       <c r="V49" s="32">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" ht="15" thickBot="1">
+      <c r="Z49" s="57">
+        <v>113</v>
+      </c>
+      <c r="AA49" s="61">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" ht="15" thickBot="1">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -7438,8 +5994,14 @@
       <c r="V50" s="33">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" ht="15" thickTop="1">
+      <c r="Z50" s="58">
+        <v>137</v>
+      </c>
+      <c r="AA50" s="62">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" ht="15" thickTop="1">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -7492,8 +6054,11 @@
       <c r="V51" s="34">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" ht="15">
+      <c r="AA51" s="60">
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" ht="15">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -7546,8 +6111,11 @@
       <c r="V52" s="32">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" ht="15">
+      <c r="AA52" s="61">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" ht="15">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -7600,8 +6168,11 @@
       <c r="V53" s="32">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" ht="15">
+      <c r="AA53" s="61">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" ht="15">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -7654,8 +6225,11 @@
       <c r="V54" s="32">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" ht="15">
+      <c r="AA54" s="61">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" ht="15">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -7708,8 +6282,11 @@
       <c r="V55" s="32">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" ht="15">
+      <c r="AA55" s="61">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" ht="15">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -7762,8 +6339,11 @@
       <c r="V56" s="32">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" ht="15">
+      <c r="AA56" s="61">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" ht="15">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -7816,8 +6396,11 @@
       <c r="V57" s="32">
         <v>2.95</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" ht="16" thickBot="1">
+      <c r="AA57" s="61">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" ht="16" thickBot="1">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -7870,8 +6453,11 @@
       <c r="V58" s="33">
         <v>3.25</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" ht="15" thickTop="1">
+      <c r="AA58" s="62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" ht="15" thickTop="1">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -7913,7 +6499,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="15">
+    <row r="60" spans="1:27" ht="15">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -7966,8 +6552,14 @@
       <c r="V60" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" ht="15">
+      <c r="Z60" s="56">
+        <v>41.2</v>
+      </c>
+      <c r="AA60" s="60">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" ht="15">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -8020,8 +6612,14 @@
       <c r="V61" s="32">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" ht="15">
+      <c r="Z61" s="57">
+        <v>46.2</v>
+      </c>
+      <c r="AA61" s="61">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" ht="15">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -8074,8 +6672,14 @@
       <c r="V62" s="32">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" ht="15">
+      <c r="Z62" s="57">
+        <v>46.8</v>
+      </c>
+      <c r="AA62" s="61">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" ht="15">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -8128,8 +6732,14 @@
       <c r="V63" s="32">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="15">
+      <c r="Z63" s="57">
+        <v>46.5</v>
+      </c>
+      <c r="AA63" s="61">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" ht="15">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -8182,8 +6792,14 @@
       <c r="V64" s="32">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" ht="15">
+      <c r="Z64" s="57">
+        <v>51.75</v>
+      </c>
+      <c r="AA64" s="61">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" ht="15">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -8236,8 +6852,14 @@
       <c r="V65" s="32">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" ht="16" thickBot="1">
+      <c r="Z65" s="57">
+        <v>56.85</v>
+      </c>
+      <c r="AA65" s="61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" ht="16" thickBot="1">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -8290,8 +6912,14 @@
       <c r="V66" s="35">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:22">
+      <c r="Z66" s="59">
+        <v>59.95</v>
+      </c>
+      <c r="AA66" s="63">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -8341,7 +6969,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:27">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -8391,7 +7019,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:27">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -8439,7 +7067,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:27">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -8489,7 +7117,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:27">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -8539,7 +7167,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:27">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -8589,7 +7217,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:27">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -8639,7 +7267,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:27">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -8689,7 +7317,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:27">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -8739,7 +7367,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="76" spans="1:22">
+    <row r="76" spans="1:27">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -8789,7 +7417,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="77" spans="1:22">
+    <row r="77" spans="1:27">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -8839,7 +7467,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="78" spans="1:22">
+    <row r="78" spans="1:27">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -8889,7 +7517,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="79" spans="1:22">
+    <row r="79" spans="1:27">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -8939,7 +7567,7 @@
         <v>25.14189</v>
       </c>
     </row>
-    <row r="80" spans="1:22">
+    <row r="80" spans="1:27">
       <c r="A80" s="5">
         <v>79</v>
       </c>

</xml_diff>